<commit_message>
Updated excel. Added 2D plot script
</commit_message>
<xml_diff>
--- a/gau_bm_new.xlsx
+++ b/gau_bm_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aodongliu/LiGroup/gaussian/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392F9454-2B54-AF4B-AE7B-78E7629AC5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B77AA75-55FF-EB4E-AA5F-7DBC9737BCFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="2" xr2:uid="{FDC61512-9885-E840-A5B5-8D65FB928F9E}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="149">
   <si>
     <t>prot-sp</t>
   </si>
@@ -6112,19 +6112,22 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:M65"/>
+  <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="135" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -6410,26 +6413,32 @@
         <f>F10*(H10^4) + G10*(I10^4) + (F10+G10)*(H10^2)*(I10^2)</f>
         <v>198575000000</v>
       </c>
-      <c r="L10" s="2" t="e">
+      <c r="L10" s="2">
         <f>K10/K11</f>
-        <v>#DIV/0!</v>
+        <v>0.27902983472848253</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="10"/>
+      <c r="B11" s="2">
+        <v>-113.832913180015</v>
+      </c>
       <c r="C11" s="2">
         <v>-113.83291364030001</v>
       </c>
       <c r="D11" s="2">
         <f>B11-C11</f>
-        <v>113.83291364030001</v>
+        <v>4.6028500833017461E-7</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="F11" s="2">
+        <v>201</v>
+      </c>
+      <c r="G11" s="2">
+        <v>4469</v>
+      </c>
       <c r="H11" s="2">
         <f>B8</f>
         <v>170</v>
@@ -6441,11 +6450,11 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2">
         <f>F11*(H11^4) + G11*(I11^4) + (F11+G11)*(H11^2)*(I11^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="2" t="e">
+        <v>711662250000</v>
+      </c>
+      <c r="L11" s="2">
         <f>K11/K11</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -6575,26 +6584,32 @@
         <f>F16*(H16^4) + G16*(I16^4) + (F16+G16)*(H16^2)*(I16^2)</f>
         <v>119287039744</v>
       </c>
-      <c r="L16" s="2" t="e">
+      <c r="L16" s="2">
         <f>K16/K17</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.22548938905606208</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="10"/>
+      <c r="B17" s="2">
+        <v>-113.832874956513</v>
+      </c>
       <c r="C17" s="2">
         <v>-113.8328754166</v>
       </c>
       <c r="D17" s="2">
         <f>B17-C17</f>
-        <v>113.8328754166</v>
+        <v>4.600870084914277E-7</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="F17" s="2">
+        <v>200</v>
+      </c>
+      <c r="G17" s="2">
+        <v>5329</v>
+      </c>
       <c r="H17" s="2">
         <f>B14</f>
         <v>170</v>
@@ -6606,14 +6621,14 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2">
         <f>F17*(H17^4) + G17*(I17^4) + (F17+G17)*(H17^2)*(I17^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="2" t="e">
+        <v>529013982624</v>
+      </c>
+      <c r="L17" s="2">
         <f>K17/K17</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -6626,11 +6641,8 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
-      <c r="M18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -6644,7 +6656,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -6658,7 +6670,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -6672,7 +6684,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -6686,7 +6698,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -6700,7 +6712,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>3</v>
       </c>
@@ -6722,7 +6734,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>134</v>
       </c>
@@ -6744,7 +6756,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
@@ -6778,7 +6790,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>15</v>
       </c>
@@ -6812,26 +6824,32 @@
         <f>F27*(H27^4) + G27*(I27^4) + (F27+G27)*(H27^2)*(I27^2)</f>
         <v>19049755600</v>
       </c>
-      <c r="L27" s="2" t="e">
+      <c r="L27" s="2">
         <f>K27/K28</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+        <v>9.3516546103713044E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="10"/>
+      <c r="B28" s="2">
+        <v>-113.82369742453599</v>
+      </c>
       <c r="C28" s="2">
         <v>-113.8236975034</v>
       </c>
       <c r="D28" s="2">
         <f>B28-C28</f>
-        <v>113.8236975034</v>
+        <v>7.8864005104151147E-8</v>
       </c>
       <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="F28" s="2">
+        <v>147</v>
+      </c>
+      <c r="G28" s="2">
+        <v>2606</v>
+      </c>
       <c r="H28" s="2">
         <f>B25</f>
         <v>88</v>
@@ -6843,14 +6861,14 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2">
         <f>F28*(H28^4) + G28*(I28^4) + (F28+G28)*(H28^2)*(I28^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L28" s="2" t="e">
+        <v>203704653280</v>
+      </c>
+      <c r="L28" s="2">
         <f>K28/K28</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -6864,7 +6882,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>3</v>
       </c>
@@ -6886,7 +6904,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>134</v>
       </c>
@@ -6909,7 +6927,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
@@ -6977,26 +6995,32 @@
         <f>F33*(H33^4) + G33*(I33^4) + (F33+G33)*(H33^2)*(I33^2)</f>
         <v>15313673984</v>
       </c>
-      <c r="L33" s="2" t="e">
+      <c r="L33" s="2">
         <f>K33/K34</f>
-        <v>#DIV/0!</v>
+        <v>0.10963708566587139</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="10"/>
+      <c r="B34" s="2">
+        <v>-113.823692323081</v>
+      </c>
       <c r="C34" s="2">
         <v>-113.8236924019</v>
       </c>
       <c r="D34" s="2">
         <f>B34-C34</f>
-        <v>113.8236924019</v>
+        <v>7.8818999327268102E-8</v>
       </c>
       <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="F34" s="2">
+        <v>147</v>
+      </c>
+      <c r="G34" s="2">
+        <v>3104</v>
+      </c>
       <c r="H34" s="2">
         <f>B31</f>
         <v>88</v>
@@ -7008,11 +7032,11 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2">
         <f>F34*(H34^4) + G34*(I34^4) + (F34+G34)*(H34^2)*(I34^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L34" s="2" t="e">
+        <v>139676040192</v>
+      </c>
+      <c r="L34" s="2">
         <f>K34/K34</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
@@ -7142,26 +7166,32 @@
         <f>F39*(H39^4) + G39*(I39^4) + (F39+G39)*(H39^2)*(I39^2)</f>
         <v>10208058000</v>
       </c>
-      <c r="L39" s="2" t="e">
+      <c r="L39" s="2">
         <f>K39/K40</f>
-        <v>#DIV/0!</v>
+        <v>0.11890023313771203</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B40" s="10"/>
+      <c r="B40" s="2">
+        <v>-113.82365677605701</v>
+      </c>
       <c r="C40" s="2">
         <v>-113.8236568547</v>
       </c>
       <c r="D40" s="2">
         <f>B40-C40</f>
-        <v>113.8236568547</v>
+        <v>7.8642997891620325E-8</v>
       </c>
       <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
+      <c r="F40" s="2">
+        <v>147</v>
+      </c>
+      <c r="G40" s="2">
+        <v>3577</v>
+      </c>
       <c r="H40" s="2">
         <f>B37</f>
         <v>88</v>
@@ -7173,11 +7203,11 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2">
         <f>F40*(H40^4) + G40*(I40^4) + (F40+G40)*(H40^2)*(I40^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L40" s="2" t="e">
+        <v>85853978000</v>
+      </c>
+      <c r="L40" s="2">
         <f>K40/K40</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
@@ -7376,26 +7406,32 @@
         <f>F50*(H50^4) + G50*(I50^4) + (F50+G50)*(H50^2)*(I50^2)</f>
         <v>4980185600</v>
       </c>
-      <c r="L50" s="2" t="e">
+      <c r="L50" s="2">
         <f>K50/K51</f>
-        <v>#DIV/0!</v>
+        <v>6.3328810349712869E-2</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="10"/>
+      <c r="B51" s="2">
+        <v>-113.790809874118</v>
+      </c>
       <c r="C51" s="2">
         <v>-113.790809873</v>
       </c>
       <c r="D51" s="2">
         <f>B51-C51</f>
-        <v>113.790809873</v>
+        <v>-1.117996362154372E-9</v>
       </c>
       <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
+      <c r="F51" s="2">
+        <v>111</v>
+      </c>
+      <c r="G51" s="2">
+        <v>2046</v>
+      </c>
       <c r="H51" s="2">
         <f>B48</f>
         <v>38</v>
@@ -7407,11 +7443,11 @@
       <c r="J51" s="2"/>
       <c r="K51" s="2">
         <f>F51*(H51^4) + G51*(I51^4) + (F51+G51)*(H51^2)*(I51^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L51" s="2" t="e">
+        <v>78640125600</v>
+      </c>
+      <c r="L51" s="2">
         <f>K51/K51</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -7541,26 +7577,32 @@
         <f>F56*(H56^4) + G56*(I56^4) + (F56+G56)*(H56^2)*(I56^2)</f>
         <v>2518751664</v>
       </c>
-      <c r="L56" s="2" t="e">
+      <c r="L56" s="2">
         <f>K56/K57</f>
-        <v>#DIV/0!</v>
+        <v>5.5605813802770604E-2</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B57" s="10"/>
+      <c r="B57" s="2">
+        <v>-113.790803416945</v>
+      </c>
       <c r="C57" s="2">
         <v>-113.7908034158</v>
       </c>
       <c r="D57" s="2">
         <f>B57-C57</f>
-        <v>113.7908034158</v>
+        <v>-1.1449969861132558E-9</v>
       </c>
       <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
+      <c r="F57" s="2">
+        <v>111</v>
+      </c>
+      <c r="G57" s="2">
+        <v>2450</v>
+      </c>
       <c r="H57" s="2">
         <f>B54</f>
         <v>38</v>
@@ -7572,11 +7614,11 @@
       <c r="J57" s="2"/>
       <c r="K57" s="2">
         <f>F57*(H57^4) + G57*(I57^4) + (F57+G57)*(H57^2)*(I57^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L57" s="2" t="e">
+        <v>45296552496</v>
+      </c>
+      <c r="L57" s="2">
         <f>K57/K57</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
@@ -7706,26 +7748,32 @@
         <f>F62*(H62^4) + G62*(I62^4) + (F62+G62)*(H62^2)*(I62^2)</f>
         <v>1140624000</v>
       </c>
-      <c r="L62" s="2" t="e">
+      <c r="L62" s="2">
         <f>K62/K63</f>
-        <v>#DIV/0!</v>
+        <v>5.8042300591002502E-2</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B63" s="2"/>
+      <c r="B63" s="2">
+        <v>-113.790762537028</v>
+      </c>
       <c r="C63" s="2">
         <v>-113.7907625359</v>
       </c>
       <c r="D63" s="2">
         <f>B63-C63</f>
-        <v>113.7907625359</v>
+        <v>-1.1280008038738742E-9</v>
       </c>
       <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
+      <c r="F63" s="2">
+        <v>111</v>
+      </c>
+      <c r="G63" s="2">
+        <v>2533</v>
+      </c>
       <c r="H63" s="2">
         <f>B60</f>
         <v>38</v>
@@ -7737,11 +7785,11 @@
       <c r="J63" s="2"/>
       <c r="K63" s="2">
         <f>F63*(H63^4) + G63*(I63^4) + (F63+G63)*(H63^2)*(I63^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L63" s="2" t="e">
+        <v>19651598720</v>
+      </c>
+      <c r="L63" s="2">
         <f>K63/K63</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
@@ -7772,6 +7820,9 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L68" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7782,7 +7833,7 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12027,8 +12078,8 @@
   </sheetPr>
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="135" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12152,26 +12203,32 @@
         <f>F4*(H4^4) + G4*(I4^4) + (F4+G4)*(H4^2)*(I4^2)</f>
         <v>36495013763</v>
       </c>
-      <c r="L4" s="2" t="e">
+      <c r="L4" s="2">
         <f>K4/K5</f>
-        <v>#DIV/0!</v>
+        <v>0.3046880156214084</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>-92.874315234199699</v>
+      </c>
       <c r="C5" s="2">
         <v>-92.874315441600004</v>
       </c>
       <c r="D5" s="2">
         <f>B5-C5</f>
-        <v>92.874315441600004</v>
+        <v>2.0740030493016093E-7</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="F5" s="2">
+        <v>112</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2569</v>
+      </c>
       <c r="H5" s="2">
         <f>B2</f>
         <v>140</v>
@@ -12183,11 +12240,11 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2">
         <f>F5*(H5^4) + G5*(I5^4) + (F5+G5)*(H5^2)*(I5^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="2" t="e">
+        <v>119778304009</v>
+      </c>
+      <c r="L5" s="2">
         <f>K5/K5</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -12482,26 +12539,32 @@
         <f>F16*(H16^4) + G16*(I16^4) + (F16+G16)*(H16^2)*(I16^2)</f>
         <v>36871074331</v>
       </c>
-      <c r="L16" s="2" t="e">
+      <c r="L16" s="2">
         <f>K16/K17</f>
-        <v>#DIV/0!</v>
+        <v>0.45593116051511634</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2">
+        <v>-92.874297479723694</v>
+      </c>
       <c r="C17" s="2">
         <v>-92.874297687099997</v>
       </c>
       <c r="D17" s="2">
         <f>B17-C17</f>
-        <v>92.874297687099997</v>
+        <v>2.0737630279654695E-7</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="F17" s="2">
+        <v>111</v>
+      </c>
+      <c r="G17" s="2">
+        <v>3482</v>
+      </c>
       <c r="H17" s="2">
         <f>B14</f>
         <v>140</v>
@@ -12513,11 +12576,11 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2">
         <f>F17*(H17^4) + G17*(I17^4) + (F17+G17)*(H17^2)*(I17^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="2" t="e">
+        <v>80869827562</v>
+      </c>
+      <c r="L17" s="2">
         <f>K17/K17</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -12719,26 +12782,32 @@
         <f>F27*(H27^4) + G27*(I27^4) + (F27+G27)*(H27^2)*(I27^2)</f>
         <v>4123154200</v>
       </c>
-      <c r="L27" s="2" t="e">
+      <c r="L27" s="2">
         <f>K27/K28</f>
-        <v>#DIV/0!</v>
+        <v>0.17047655947307244</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2">
+        <v>-92.867904124437203</v>
+      </c>
       <c r="C28" s="2">
         <v>-92.867904256599999</v>
       </c>
       <c r="D28" s="2">
         <f>B28-C28</f>
-        <v>92.867904256599999</v>
+        <v>1.3216279626249161E-7</v>
       </c>
       <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="F28" s="2">
+        <v>99</v>
+      </c>
+      <c r="G28" s="2">
+        <v>2185</v>
+      </c>
       <c r="H28" s="2">
         <f>B25</f>
         <v>74</v>
@@ -12750,11 +12819,11 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2">
         <f>F28*(H28^4) + G28*(I28^4) + (F28+G28)*(H28^2)*(I28^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L28" s="2" t="e">
+        <v>24186047705</v>
+      </c>
+      <c r="L28" s="2">
         <f>K28/K28</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -12884,26 +12953,32 @@
         <f>F33*(H33^4) + G33*(I33^4) + (F33+G33)*(H33^2)*(I33^2)</f>
         <v>3170963328</v>
       </c>
-      <c r="L33" s="2" t="e">
+      <c r="L33" s="2">
         <f>K33/K34</f>
-        <v>#DIV/0!</v>
+        <v>0.17933206982198335</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="2"/>
+      <c r="B34" s="2">
+        <v>-92.867903817892497</v>
+      </c>
       <c r="C34" s="2">
         <v>-92.867903950100001</v>
       </c>
       <c r="D34" s="2">
         <f>B34-C34</f>
-        <v>92.867903950100001</v>
+        <v>1.3220750361142564E-7</v>
       </c>
       <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="F34" s="2">
+        <v>99</v>
+      </c>
+      <c r="G34" s="2">
+        <v>2479</v>
+      </c>
       <c r="H34" s="2">
         <f>B31</f>
         <v>74</v>
@@ -12915,11 +12990,11 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2">
         <f>F34*(H34^4) + G34*(I34^4) + (F34+G34)*(H34^2)*(I34^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L34" s="2" t="e">
+        <v>17682076224</v>
+      </c>
+      <c r="L34" s="2">
         <f>K34/K34</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
@@ -13049,26 +13124,32 @@
         <f>F39*(H39^4) + G39*(I39^4) + (F39+G39)*(H39^2)*(I39^2)</f>
         <v>2740561900</v>
       </c>
-      <c r="L39" s="2" t="e">
+      <c r="L39" s="2">
         <f>K39/K40</f>
-        <v>#DIV/0!</v>
+        <v>0.21255548155427528</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B40" s="10"/>
+      <c r="B40" s="2">
+        <v>-92.867886831546897</v>
+      </c>
       <c r="C40" s="2">
         <v>-92.867886963800004</v>
       </c>
       <c r="D40" s="2">
         <f>B40-C40</f>
-        <v>92.867886963800004</v>
+        <v>1.3225310624420672E-7</v>
       </c>
       <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
+      <c r="F40" s="2">
+        <v>99</v>
+      </c>
+      <c r="G40" s="2">
+        <v>3034</v>
+      </c>
       <c r="H40" s="2">
         <f>B37</f>
         <v>74</v>
@@ -13080,11 +13161,11 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2">
         <f>F40*(H40^4) + G40*(I40^4) + (F40+G40)*(H40^2)*(I40^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L40" s="2" t="e">
+        <v>12893395550</v>
+      </c>
+      <c r="L40" s="2">
         <f>K40/K40</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
@@ -13283,26 +13364,32 @@
         <f>F50*(H50^4) + G50*(I50^4) + (F50+G50)*(H50^2)*(I50^2)</f>
         <v>495424648</v>
       </c>
-      <c r="L50" s="2" t="e">
+      <c r="L50" s="2">
         <f>K50/K51</f>
-        <v>#DIV/0!</v>
+        <v>6.7068254517031439E-2</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="2"/>
+      <c r="B51" s="2">
+        <v>-92.844552683229907</v>
+      </c>
       <c r="C51" s="2">
         <v>-92.844552682</v>
       </c>
       <c r="D51" s="2">
         <f>B51-C51</f>
-        <v>92.844552682</v>
+        <v>-1.2299068430365878E-9</v>
       </c>
       <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
+      <c r="F51" s="2">
+        <v>87</v>
+      </c>
+      <c r="G51" s="2">
+        <v>2126</v>
+      </c>
       <c r="H51" s="2">
         <f>B48</f>
         <v>33</v>
@@ -13314,11 +13401,11 @@
       <c r="J51" s="2"/>
       <c r="K51" s="2">
         <f>F51*(H51^4) + G51*(I51^4) + (F51+G51)*(H51^2)*(I51^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L51" s="2" t="e">
+        <v>7386872546</v>
+      </c>
+      <c r="L51" s="2">
         <f>K51/K51</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -13448,26 +13535,32 @@
         <f>F56*(H56^4) + G56*(I56^4) + (F56+G56)*(H56^2)*(I56^2)</f>
         <v>288796833</v>
       </c>
-      <c r="L56" s="2" t="e">
+      <c r="L56" s="2">
         <f>K56/K57</f>
-        <v>#DIV/0!</v>
+        <v>7.2207029589082788E-2</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B57" s="2"/>
+      <c r="B57" s="2">
+        <v>-92.844550440394002</v>
+      </c>
       <c r="C57" s="2">
         <v>-92.844550439200006</v>
       </c>
       <c r="D57" s="2">
         <f>B57-C57</f>
-        <v>92.844550439200006</v>
+        <v>-1.1939960131712724E-9</v>
       </c>
       <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
+      <c r="F57" s="2">
+        <v>87</v>
+      </c>
+      <c r="G57" s="2">
+        <v>2129</v>
+      </c>
       <c r="H57" s="2">
         <f>B54</f>
         <v>33</v>
@@ -13479,11 +13572,11 @@
       <c r="J57" s="2"/>
       <c r="K57" s="2">
         <f>F57*(H57^4) + G57*(I57^4) + (F57+G57)*(H57^2)*(I57^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L57" s="2" t="e">
+        <v>3999566727</v>
+      </c>
+      <c r="L57" s="2">
         <f>K57/K57</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
@@ -13613,26 +13706,32 @@
         <f>F62*(H62^4) + G62*(I62^4) + (F62+G62)*(H62^2)*(I62^2)</f>
         <v>157075440</v>
       </c>
-      <c r="L62" s="2" t="e">
+      <c r="L62" s="2">
         <f>K62/K63</f>
-        <v>#DIV/0!</v>
+        <v>7.1795387582681544E-2</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B63" s="2"/>
+      <c r="B63" s="2">
+        <v>-92.844531342948798</v>
+      </c>
       <c r="C63" s="2">
         <v>-92.844531341700005</v>
       </c>
       <c r="D63" s="2">
         <f>B63-C63</f>
-        <v>92.844531341700005</v>
+        <v>-1.2487930689530913E-9</v>
       </c>
       <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
+      <c r="F63" s="2">
+        <v>87</v>
+      </c>
+      <c r="G63" s="2">
+        <v>2377</v>
+      </c>
       <c r="H63" s="2">
         <f>B60</f>
         <v>33</v>
@@ -13644,11 +13743,11 @@
       <c r="J63" s="2"/>
       <c r="K63" s="2">
         <f>F63*(H63^4) + G63*(I63^4) + (F63+G63)*(H63^2)*(I63^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L63" s="2" t="e">
+        <v>2187820768</v>
+      </c>
+      <c r="L63" s="2">
         <f>K63/K63</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
@@ -13691,8 +13790,8 @@
   </sheetPr>
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="135" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="135" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13986,26 +14085,32 @@
         <f>F10*(H10^4) + G10*(I10^4) + (F10+G10)*(H10^2)*(I10^2)</f>
         <v>21432750000</v>
       </c>
-      <c r="L10" s="2" t="e">
+      <c r="L10" s="2">
         <f>K10/K11</f>
-        <v>#DIV/0!</v>
+        <v>0.75651230101302458</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="10"/>
+      <c r="B11" s="2">
+        <v>-199.55232171020799</v>
+      </c>
       <c r="C11" s="2">
         <v>-199.5523218056</v>
       </c>
       <c r="D11" s="2">
         <f>B11-C11</f>
-        <v>199.5523218056</v>
+        <v>9.5392010734940413E-8</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="F11" s="2">
+        <v>38</v>
+      </c>
+      <c r="G11" s="2">
+        <v>708</v>
+      </c>
       <c r="H11" s="2">
         <f>B8</f>
         <v>140</v>
@@ -14017,11 +14122,11 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2">
         <f>F11*(H11^4) + G11*(I11^4) + (F11+G11)*(H11^2)*(I11^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="2" t="e">
+        <v>28331000000</v>
+      </c>
+      <c r="L11" s="2">
         <f>K11/K11</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -14151,26 +14256,32 @@
         <f>F16*(H16^4) + G16*(I16^4) + (F16+G16)*(H16^2)*(I16^2)</f>
         <v>14586359076</v>
       </c>
-      <c r="L16" s="2" t="e">
+      <c r="L16" s="2">
         <f>K16/K17</f>
-        <v>#DIV/0!</v>
+        <v>0.59278831641488738</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2">
+        <v>-199.55232159262101</v>
+      </c>
       <c r="C17" s="2">
         <v>-199.55232168800001</v>
       </c>
       <c r="D17" s="2">
         <f>B17-C17</f>
-        <v>199.55232168800001</v>
+        <v>9.5378993592021288E-8</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="F17" s="2">
+        <v>36</v>
+      </c>
+      <c r="G17" s="2">
+        <v>977</v>
+      </c>
       <c r="H17" s="2">
         <f>B14</f>
         <v>140</v>
@@ -14182,11 +14293,11 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2">
         <f>F17*(H17^4) + G17*(I17^4) + (F17+G17)*(H17^2)*(I17^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="2" t="e">
+        <v>24606353857</v>
+      </c>
+      <c r="L17" s="2">
         <f>K17/K17</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -14969,26 +15080,32 @@
         <f>F50*(H50^4) + G50*(I50^4) + (F50+G50)*(H50^2)*(I50^2)</f>
         <v>374589368</v>
       </c>
-      <c r="L50" s="2" t="e">
+      <c r="L50" s="2">
         <f>K50/K51</f>
-        <v>#DIV/0!</v>
+        <v>0.1521508849243868</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="2"/>
+      <c r="B51" s="2">
+        <v>-199.443038266212</v>
+      </c>
       <c r="C51" s="2">
         <v>-199.44303827030001</v>
       </c>
       <c r="D51" s="2">
         <f>B51-C51</f>
-        <v>199.44303827030001</v>
+        <v>4.08800815421273E-9</v>
       </c>
       <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
+      <c r="F51" s="2">
+        <v>36</v>
+      </c>
+      <c r="G51" s="2">
+        <v>703</v>
+      </c>
       <c r="H51" s="2">
         <f>B48</f>
         <v>33</v>
@@ -15000,11 +15117,11 @@
       <c r="J51" s="2"/>
       <c r="K51" s="2">
         <f>F51*(H51^4) + G51*(I51^4) + (F51+G51)*(H51^2)*(I51^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L51" s="2" t="e">
+        <v>2461959838</v>
+      </c>
+      <c r="L51" s="2">
         <f>K51/K51</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -15134,26 +15251,32 @@
         <f>F56*(H56^4) + G56*(I56^4) + (F56+G56)*(H56^2)*(I56^2)</f>
         <v>249235623</v>
       </c>
-      <c r="L56" s="2" t="e">
+      <c r="L56" s="2">
         <f>K56/K57</f>
-        <v>#DIV/0!</v>
+        <v>0.18599711445976275</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B57" s="2"/>
+      <c r="B57" s="2">
+        <v>-199.443038266212</v>
+      </c>
       <c r="C57" s="2">
         <v>-199.44303827030001</v>
       </c>
       <c r="D57" s="2">
         <f>B57-C57</f>
-        <v>199.44303827030001</v>
+        <v>4.08800815421273E-9</v>
       </c>
       <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
+      <c r="F57" s="2">
+        <v>36</v>
+      </c>
+      <c r="G57" s="2">
+        <v>705</v>
+      </c>
       <c r="H57" s="2">
         <f>B54</f>
         <v>33</v>
@@ -15165,11 +15288,11 @@
       <c r="J57" s="2"/>
       <c r="K57" s="2">
         <f>F57*(H57^4) + G57*(I57^4) + (F57+G57)*(H57^2)*(I57^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L57" s="2" t="e">
+        <v>1339997256</v>
+      </c>
+      <c r="L57" s="2">
         <f>K57/K57</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
@@ -15299,9 +15422,9 @@
         <f>F62*(H62^4) + G62*(I62^4) + (F62+G62)*(H62^2)*(I62^2)</f>
         <v>83773568</v>
       </c>
-      <c r="L62" s="2" t="e">
+      <c r="L62" s="2">
         <f>K62/K63</f>
-        <v>#DIV/0!</v>
+        <v>0.1007870091898847</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
@@ -15319,8 +15442,12 @@
         <v>4.0999736938829301E-9</v>
       </c>
       <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
+      <c r="F63" s="2">
+        <v>36</v>
+      </c>
+      <c r="G63" s="2">
+        <v>897</v>
+      </c>
       <c r="H63" s="2">
         <f>B60</f>
         <v>33</v>
@@ -15332,11 +15459,11 @@
       <c r="J63" s="2"/>
       <c r="K63" s="2">
         <f>F63*(H63^4) + G63*(I63^4) + (F63+G63)*(H63^2)*(I63^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L63" s="2" t="e">
+        <v>831194106</v>
+      </c>
+      <c r="L63" s="2">
         <f>K63/K63</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
@@ -15375,7 +15502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3327EFD-6666-8440-8A02-3CF6012FB162}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="162" zoomScaleNormal="195" workbookViewId="0">
+    <sheetView zoomScale="162" zoomScaleNormal="195" workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
@@ -16400,7 +16527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82990E15-10D1-3848-B6B2-340B2D9BA8E7}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="206" workbookViewId="0">
+    <sheetView zoomScale="103" workbookViewId="0">
       <selection activeCell="E31" sqref="E31:E32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
All calculations results added. 2D plot completed
</commit_message>
<xml_diff>
--- a/gau_bm_new.xlsx
+++ b/gau_bm_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aodongliu/LiGroup/gaussian/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B77AA75-55FF-EB4E-AA5F-7DBC9737BCFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1197A1AD-30BB-3045-8B88-94E59E9D28E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="2" xr2:uid="{FDC61512-9885-E840-A5B5-8D65FB928F9E}"/>
+    <workbookView xWindow="60" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="1" xr2:uid="{FDC61512-9885-E840-A5B5-8D65FB928F9E}"/>
   </bookViews>
   <sheets>
     <sheet name="COH2 NEW" sheetId="18" r:id="rId1"/>
@@ -6114,8 +6114,8 @@
   </sheetPr>
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7825,6 +7825,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -8503,6 +8504,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -8798,6 +8800,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -9344,6 +9347,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -9352,7 +9356,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="236" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9540,6 +9544,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -9739,6 +9744,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -9938,6 +9944,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -10137,6 +10144,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -11532,6 +11540,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -12067,6 +12076,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -12078,8 +12088,8 @@
   </sheetPr>
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12374,26 +12384,32 @@
         <f>F10*(H10^4) + G10*(I10^4) + (F10+G10)*(H10^2)*(I10^2)</f>
         <v>31518750000</v>
       </c>
-      <c r="L10" s="2" t="e">
+      <c r="L10" s="2">
         <f>K10/K11</f>
-        <v>#DIV/0!</v>
+        <v>0.3231603505895706</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>-92.874314976384497</v>
+      </c>
       <c r="C11" s="2">
         <v>-92.874315183899995</v>
       </c>
       <c r="D11" s="2">
         <f>B11-C11</f>
-        <v>92.874315183899995</v>
+        <v>2.0751549811848236E-7</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="F11" s="2">
+        <v>111</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2869</v>
+      </c>
       <c r="H11" s="2">
         <f>B8</f>
         <v>140</v>
@@ -12405,11 +12421,11 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2">
         <f>F11*(H11^4) + G11*(I11^4) + (F11+G11)*(H11^2)*(I11^2)</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="2" t="e">
+        <v>97532850000</v>
+      </c>
+      <c r="L11" s="2">
         <f>K11/K11</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -13780,6 +13796,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -13790,8 +13807,8 @@
   </sheetPr>
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="135" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="C34" zoomScale="141" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15495,6 +15512,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -16125,6 +16143,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -16520,6 +16539,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -17375,6 +17395,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -17770,6 +17791,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -18831,6 +18853,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -19226,5 +19249,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add new CQ data to excel
</commit_message>
<xml_diff>
--- a/gau_bm_new.xlsx
+++ b/gau_bm_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aodongliu/LiGroup/gaussian/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1197A1AD-30BB-3045-8B88-94E59E9D28E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391BA933-56C0-7641-B245-38F3980806E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="1" xr2:uid="{FDC61512-9885-E840-A5B5-8D65FB928F9E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="13" xr2:uid="{FDC61512-9885-E840-A5B5-8D65FB928F9E}"/>
   </bookViews>
   <sheets>
     <sheet name="COH2 NEW" sheetId="18" r:id="rId1"/>
@@ -22,15 +22,13 @@
     <sheet name="HCN CC" sheetId="14" r:id="rId7"/>
     <sheet name="FHF-" sheetId="4" r:id="rId8"/>
     <sheet name="FHF CC" sheetId="15" r:id="rId9"/>
-    <sheet name="FHF- (2)" sheetId="16" r:id="rId10"/>
-    <sheet name="FHF CC (2)" sheetId="17" r:id="rId11"/>
-    <sheet name="CC" sheetId="12" r:id="rId12"/>
-    <sheet name="4H2O+ Eigen" sheetId="5" r:id="rId13"/>
-    <sheet name="4H2O+ Ring" sheetId="6" r:id="rId14"/>
-    <sheet name="4H2O+ cisZundel" sheetId="7" r:id="rId15"/>
-    <sheet name="4H2O+ transZundel" sheetId="8" r:id="rId16"/>
-    <sheet name="MaxCom" sheetId="10" r:id="rId17"/>
-    <sheet name="MaxCom Plot" sheetId="11" r:id="rId18"/>
+    <sheet name="CC" sheetId="12" r:id="rId10"/>
+    <sheet name="4H2O+ Eigen" sheetId="5" r:id="rId11"/>
+    <sheet name="4H2O+ Ring" sheetId="6" r:id="rId12"/>
+    <sheet name="4H2O+ cisZundel" sheetId="7" r:id="rId13"/>
+    <sheet name="4H2O+ transZundel" sheetId="8" r:id="rId14"/>
+    <sheet name="MaxCom" sheetId="10" r:id="rId15"/>
+    <sheet name="MaxCom Plot" sheetId="11" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="149">
   <si>
     <t>prot-sp</t>
   </si>
@@ -458,16 +456,10 @@
     <t>cc-pvtz (5d, 7f)</t>
   </si>
   <si>
-    <t xml:space="preserve">pb4-d </t>
-  </si>
-  <si>
     <t>pb4-d</t>
   </si>
   <si>
     <t xml:space="preserve">pb4-f1 </t>
-  </si>
-  <si>
-    <t>pb4-f2</t>
   </si>
   <si>
     <t xml:space="preserve">pb4-f2 </t>
@@ -499,12 +491,18 @@
   <si>
     <t>Speedup</t>
   </si>
+  <si>
+    <t>ls</t>
+  </si>
+  <si>
+    <t>hatz</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -534,12 +532,6 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFC5C5C5"/>
       <name val="Menlo"/>
       <family val="2"/>
     </font>
@@ -578,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -593,7 +585,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6114,8 +6105,8 @@
   </sheetPr>
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="A25" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6154,13 +6145,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" s="3">
         <v>170</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D2" s="3">
         <v>74</v>
@@ -6189,23 +6180,23 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -6324,14 +6315,14 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B8" s="3">
         <f>B2</f>
         <v>170</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D8" s="3">
         <v>60</v>
@@ -6360,23 +6351,23 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -6459,7 +6450,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="10"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -6495,14 +6486,14 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B14" s="3">
         <f>B2</f>
         <v>170</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D14" s="3">
         <v>46</v>
@@ -6531,23 +6522,23 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -6584,9 +6575,9 @@
         <f>F16*(H16^4) + G16*(I16^4) + (F16+G16)*(H16^2)*(I16^2)</f>
         <v>119287039744</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="2" t="e">
         <f>K16/K17</f>
-        <v>0.22548938905606208</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -6607,8 +6598,8 @@
       <c r="F17" s="2">
         <v>200</v>
       </c>
-      <c r="G17" s="2">
-        <v>5329</v>
+      <c r="G17" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="H17" s="2">
         <f>B14</f>
@@ -6619,13 +6610,13 @@
         <v>46</v>
       </c>
       <c r="J17" s="2"/>
-      <c r="K17" s="2">
+      <c r="K17" s="2" t="e">
         <f>F17*(H17^4) + G17*(I17^4) + (F17+G17)*(H17^2)*(I17^2)</f>
-        <v>529013982624</v>
-      </c>
-      <c r="L17" s="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L17" s="2" t="e">
         <f>K17/K17</f>
-        <v>1</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -6742,7 +6733,7 @@
         <v>88</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D25" s="3">
         <v>74</v>
@@ -6771,23 +6762,23 @@
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -6913,7 +6904,7 @@
         <v>88</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D31" s="3">
         <v>60</v>
@@ -6942,23 +6933,23 @@
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I32" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -7041,7 +7032,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
-      <c r="B35" s="10"/>
+      <c r="B35" s="9"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -7084,7 +7075,7 @@
         <v>88</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D37" s="3">
         <v>46</v>
@@ -7113,23 +7104,23 @@
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
@@ -7318,13 +7309,13 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B48" s="3">
         <v>38</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D48" s="3">
         <v>74</v>
@@ -7353,23 +7344,23 @@
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I49" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J49" s="2"/>
       <c r="K49" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
@@ -7488,14 +7479,14 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B54" s="3">
         <f>B48</f>
         <v>38</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D54" s="3">
         <v>60</v>
@@ -7524,23 +7515,23 @@
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I55" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G55" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J55" s="2"/>
       <c r="K55" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
@@ -7623,7 +7614,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
-      <c r="B58" s="10"/>
+      <c r="B58" s="9"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -7659,14 +7650,14 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B60" s="3">
         <f>B48</f>
         <v>38</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D60" s="3">
         <v>46</v>
@@ -7695,23 +7686,23 @@
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I61" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G61" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I61" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J61" s="2"/>
       <c r="K61" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
@@ -7830,985 +7821,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{386DEE7F-07BB-FD4A-BF1A-86C27F75DC1E}">
-  <dimension ref="A1:M50"/>
-  <sheetViews>
-    <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B2" s="3">
-        <v>74</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D2" s="3">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="2">
-        <v>-199.527422194406</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2">
-        <f>ABS(B4-C4)</f>
-        <v>199.527422194406</v>
-      </c>
-      <c r="E4" s="2">
-        <v>33</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2">
-        <v>-199.52915136300001</v>
-      </c>
-      <c r="H4" s="2">
-        <f>ABS(G4-B4)</f>
-        <v>1.7291685940108437E-3</v>
-      </c>
-      <c r="I4">
-        <f>E6/E4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="8">
-        <v>-199.52742219440501</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2">
-        <f>ABS(B6-C6)</f>
-        <v>199.52742219440501</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2">
-        <v>5</v>
-      </c>
-      <c r="G6" s="2">
-        <v>-199.52915136300001</v>
-      </c>
-      <c r="H6" s="2">
-        <f t="shared" ref="H6" si="0">ABS(G6-B6)</f>
-        <v>1.7291685950056035E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B9" s="3">
-        <v>140</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D9" s="3">
-        <v>37</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="8">
-        <v>-199.55232171019</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2">
-        <f>ABS(B11-C11)</f>
-        <v>199.55232171019</v>
-      </c>
-      <c r="E11" s="2">
-        <v>282</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2">
-        <v>-199.55360597550001</v>
-      </c>
-      <c r="H11" s="2">
-        <f>ABS(G11-B11)</f>
-        <v>1.2842653100051393E-3</v>
-      </c>
-      <c r="I11">
-        <f>E13/E11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="8">
-        <v>-199.55232171020799</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2">
-        <f>ABS(B13-C13)</f>
-        <v>199.55232171020799</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2">
-        <v>5</v>
-      </c>
-      <c r="G13" s="2">
-        <v>-199.55360597550001</v>
-      </c>
-      <c r="H13" s="2">
-        <f t="shared" ref="H13" si="1">ABS(G13-B13)</f>
-        <v>1.2842652920141973E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B17" s="3">
-        <v>74</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D17" s="3">
-        <v>30</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="M18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="8">
-        <v>-199.52742219440401</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2">
-        <f>ABS(B19-C19)</f>
-        <v>199.52742219440401</v>
-      </c>
-      <c r="E19" s="2">
-        <v>33</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" ht="18" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="8">
-        <v>-199.52742219440501</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2">
-        <f>ABS(B21-C21)</f>
-        <v>199.52742219440501</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2">
-        <v>5</v>
-      </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B26" s="3">
-        <v>74</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D26" s="3">
-        <v>23</v>
-      </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="18" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="8">
-        <v>-199.527421214013</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2">
-        <f>ABS(B28-C28)</f>
-        <v>199.527421214013</v>
-      </c>
-      <c r="E28" s="2">
-        <v>37</v>
-      </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2">
-        <v>-199.5291513791</v>
-      </c>
-      <c r="H28" s="2">
-        <f>ABS(G28-B28)</f>
-        <v>1.7301650869967489E-3</v>
-      </c>
-      <c r="I28">
-        <f>E30/E28</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:13" ht="18" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="8">
-        <v>-199.527421214013</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2">
-        <f>ABS(B30-C30)</f>
-        <v>199.527421214013</v>
-      </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2">
-        <v>5</v>
-      </c>
-      <c r="G30" s="2">
-        <v>-199.5291513791</v>
-      </c>
-      <c r="H30" s="2">
-        <f t="shared" ref="H30" si="2">ABS(G30-B30)</f>
-        <v>1.7301650869967489E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C32" s="4"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B35" s="3">
-        <v>33</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D35" s="3">
-        <v>23</v>
-      </c>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I36" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>15</v>
-      </c>
-      <c r="B37" s="8">
-        <v>-199.44303753080001</v>
-      </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2">
-        <f>ABS(B37-C37)</f>
-        <v>199.44303753080001</v>
-      </c>
-      <c r="E37" s="2">
-        <v>32</v>
-      </c>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2">
-        <v>-199.4434704741</v>
-      </c>
-      <c r="H37" s="2">
-        <f>ABS(G37-B37)</f>
-        <v>4.3294329998389003E-4</v>
-      </c>
-      <c r="I37">
-        <f>E39/E37</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2">
-        <f>ABS(B39-C39)</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2">
-        <v>5</v>
-      </c>
-      <c r="G39" s="2">
-        <v>-199.4434704741</v>
-      </c>
-      <c r="H39" s="2">
-        <f>ABS(G39-B39)</f>
-        <v>199.4434704741</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9974C548-22C7-6747-8B5E-DE6A710103C8}">
-  <dimension ref="A1:G18"/>
-  <sheetViews>
-    <sheetView zoomScale="182" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2">
-        <v>33</v>
-      </c>
-      <c r="C2">
-        <v>74</v>
-      </c>
-      <c r="D2">
-        <v>33</v>
-      </c>
-      <c r="E2">
-        <v>37</v>
-      </c>
-      <c r="F2">
-        <f>B2*(C2^4)+D2*(E2^4)+(C2^2)*(E2^2)*(B2+D2)</f>
-        <v>1546182825</v>
-      </c>
-      <c r="G2">
-        <f>F2/F3</f>
-        <v>0.19784172661870503</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3">
-        <v>36</v>
-      </c>
-      <c r="C3">
-        <v>74</v>
-      </c>
-      <c r="D3">
-        <v>690</v>
-      </c>
-      <c r="E3">
-        <v>37</v>
-      </c>
-      <c r="F3">
-        <f>B3*(C3^4)+D3*(E3^4)+(C3^2)*(E3^2)*(B3+D3)</f>
-        <v>7815251370</v>
-      </c>
-      <c r="G3">
-        <f>F3/F3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>129</v>
-      </c>
-      <c r="B6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" t="s">
-        <v>103</v>
-      </c>
-      <c r="E6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B7" s="2">
-        <v>53</v>
-      </c>
-      <c r="C7">
-        <v>140</v>
-      </c>
-      <c r="D7" s="2">
-        <v>53</v>
-      </c>
-      <c r="E7">
-        <v>37</v>
-      </c>
-      <c r="F7">
-        <f>B7*(C7^4)+D7*(E7^4)+(C7^2)*(E7^2)*(B7+D7)</f>
-        <v>23304044933</v>
-      </c>
-      <c r="G7">
-        <f>F7/F8</f>
-        <v>0.6509796410159987</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B8">
-        <v>38</v>
-      </c>
-      <c r="C8">
-        <v>140</v>
-      </c>
-      <c r="D8">
-        <v>703</v>
-      </c>
-      <c r="E8">
-        <v>37</v>
-      </c>
-      <c r="F8">
-        <f>B8*(C8^4)+D8*(E8^4)+(C8^2)*(E8^2)*(B8+D8)</f>
-        <v>35798423583</v>
-      </c>
-      <c r="G8">
-        <f>F8/F8</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" t="s">
-        <v>103</v>
-      </c>
-      <c r="E11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B12" s="2">
-        <v>33</v>
-      </c>
-      <c r="C12">
-        <v>74</v>
-      </c>
-      <c r="D12" s="2">
-        <v>33</v>
-      </c>
-      <c r="E12">
-        <v>30</v>
-      </c>
-      <c r="F12">
-        <f>B12*(C12^4)+D12*(E12^4)+(C12^2)*(E12^2)*(B12+D12)</f>
-        <v>1341561408</v>
-      </c>
-      <c r="G12">
-        <f>F12/F13</f>
-        <v>0.25689713272676656</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>115</v>
-      </c>
-      <c r="B13">
-        <v>36</v>
-      </c>
-      <c r="C13">
-        <v>74</v>
-      </c>
-      <c r="D13">
-        <v>691</v>
-      </c>
-      <c r="E13">
-        <v>30</v>
-      </c>
-      <c r="F13">
-        <f>B13*(C13^4)+D13*(E13^4)+(C13^2)*(E13^2)*(B13+D13)</f>
-        <v>5222173536</v>
-      </c>
-      <c r="G13">
-        <f>F13/F13</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>133</v>
-      </c>
-      <c r="B16" t="s">
-        <v>102</v>
-      </c>
-      <c r="C16" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" t="s">
-        <v>103</v>
-      </c>
-      <c r="E16" t="s">
-        <v>105</v>
-      </c>
-      <c r="F16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B17" s="2">
-        <v>37</v>
-      </c>
-      <c r="C17">
-        <v>74</v>
-      </c>
-      <c r="D17" s="2">
-        <v>37</v>
-      </c>
-      <c r="E17">
-        <v>23</v>
-      </c>
-      <c r="F17">
-        <f>B17*(C17^4)+D17*(E17^4)+(C17^2)*(E17^2)*(B17+D17)</f>
-        <v>1334220925</v>
-      </c>
-      <c r="G17">
-        <f>F17/F18</f>
-        <v>0.32094672675795921</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>115</v>
-      </c>
-      <c r="B18">
-        <v>36</v>
-      </c>
-      <c r="C18">
-        <v>74</v>
-      </c>
-      <c r="D18">
-        <v>936</v>
-      </c>
-      <c r="E18">
-        <v>23</v>
-      </c>
-      <c r="F18">
-        <f>B18*(C18^4)+D18*(E18^4)+(C18^2)*(E18^2)*(B18+D18)</f>
-        <v>4157141400</v>
-      </c>
-      <c r="G18">
-        <f>F18/F18</f>
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8C2356-22A4-2D4C-8C02-DBBF49DBB3D5}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="C17" zoomScale="193" workbookViewId="0">
+    <sheetView zoomScale="193" workbookViewId="0">
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
@@ -9351,12 +8367,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D73C6EE8-AF48-0D41-9751-DBFA9209D173}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="236" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9380,7 +8396,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>148</v>
       </c>
       <c r="B2" s="3">
         <v>335</v>
@@ -9405,137 +8421,315 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="7">
-        <v>-304.282028608622</v>
-      </c>
-      <c r="C4" s="5"/>
+      <c r="B4" s="2">
+        <v>-304.27859365971199</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-304.27859388770003</v>
+      </c>
       <c r="D4" s="2">
         <f>ABS(B4-C4)</f>
-        <v>304.282028608622</v>
-      </c>
-      <c r="E4" s="2">
-        <v>220</v>
-      </c>
+        <v>2.2798803911427967E-7</v>
+      </c>
+      <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="2">
-        <f>E5/E4</f>
-        <v>17.572727272727274</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="7">
-        <v>-304.282028608556</v>
-      </c>
-      <c r="C5" s="2"/>
+      <c r="B5" s="2">
+        <v>-304.27859365964099</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-304.27859388770003</v>
+      </c>
       <c r="D5" s="2">
         <f>ABS(B5-C5)</f>
-        <v>304.282028608556</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3866</v>
-      </c>
-      <c r="F5" s="2">
-        <v>22</v>
-      </c>
+        <v>2.2805903654443682E-7</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B373111C-524D-584A-8386-F6E20B240E5F}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView zoomScale="168" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="3">
+        <v>335</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-304.26872879850998</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-303.76549672739998</v>
+      </c>
+      <c r="D4" s="2">
+        <f>ABS(B4-C4)</f>
+        <v>0.50323207111000556</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2">
+        <v>-304.26872879845001</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-303.76549672739998</v>
+      </c>
+      <c r="D5" s="2">
+        <f>ABS(B5-C5)</f>
+        <v>0.50323207105003576</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="B10" s="2"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D0AD158-98D5-8442-AC1E-D2F5E3C7D0DC}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="3">
         <v>335</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="3">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2">
-        <v>-304.28204683004498</v>
-      </c>
+      <c r="B4" s="2">
+        <v>-304.27240443042001</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-303.67048784780002</v>
+      </c>
+      <c r="D4" s="2">
+        <f>ABS(B4-C4)</f>
+        <v>0.60191658261999237</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2">
+        <v>-304.27240443036601</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-303.67048784780002</v>
+      </c>
+      <c r="D5" s="2">
+        <f>ABS(B5-C5)</f>
+        <v>0.60191658256599112</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="B10" s="5"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="2">
-        <f>ABS(B10-C10)</f>
-        <v>304.28204683004498</v>
-      </c>
-      <c r="E10" s="2">
-        <v>199</v>
-      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2">
-        <f>E11/E10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="B11" s="5"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -9549,11 +8743,11 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B373111C-524D-584A-8386-F6E20B240E5F}">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B100792-F8E9-2145-A8FC-022CBCD50240}">
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView zoomScale="168" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="144" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9614,33 +8808,33 @@
         <v>15</v>
       </c>
       <c r="B4" s="5">
-        <v>-304.27205100816502</v>
+        <v>-304.27613652339198</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2">
         <f>ABS(B4-C4)</f>
-        <v>304.27205100816502</v>
+        <v>304.27613652339198</v>
       </c>
       <c r="E4" s="2">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
         <f>E5/E4</f>
-        <v>16.381355932203391</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+        <v>16.521367521367523</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="5">
-        <v>-304.27205100807203</v>
+      <c r="B5" s="2">
+        <v>-304.282028608556</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2">
         <f>ABS(B5-C5)</f>
-        <v>304.27205100807203</v>
+        <v>304.282028608556</v>
       </c>
       <c r="E5" s="2">
         <v>3866</v>
@@ -9706,20 +8900,20 @@
         <v>15</v>
       </c>
       <c r="B10" s="2">
-        <v>-304.272070125352</v>
+        <v>-304.27615367897698</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2">
         <f>ABS(B10-C10)</f>
-        <v>304.272070125352</v>
+        <v>304.27615367897698</v>
       </c>
       <c r="E10" s="2">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2">
         <f>E11/E10</f>
-        <v>13.817258883248732</v>
+        <v>14.155440414507773</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -9727,20 +8921,88 @@
         <v>17</v>
       </c>
       <c r="B11" s="2">
-        <v>-304.27207012530698</v>
+        <v>-304.27615367888802</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2">
         <f>ABS(B11-C11)</f>
-        <v>304.27207012530698</v>
+        <v>304.27615367888802</v>
       </c>
       <c r="E11" s="2">
-        <v>2722</v>
+        <v>2732</v>
       </c>
       <c r="F11" s="2">
         <v>22</v>
       </c>
       <c r="G11" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" s="3">
+        <v>335</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="7">
+        <v>-304.27270755958</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2">
+        <f>ABS(B21-C21)</f>
+        <v>304.27270755958</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="7">
+        <v>-304.27270755949598</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2">
+        <f>ABS(B22-C22)</f>
+        <v>304.27270755949598</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9749,406 +9011,6 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D0AD158-98D5-8442-AC1E-D2F5E3C7D0DC}">
-  <dimension ref="A1:G11"/>
-  <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="3">
-        <v>335</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="3">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="7">
-        <v>-304.27581395078602</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="2">
-        <f>ABS(B4-C4)</f>
-        <v>304.27581395078602</v>
-      </c>
-      <c r="E4" s="2">
-        <v>225</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2">
-        <f>E5/E4</f>
-        <v>17.182222222222222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="7">
-        <v>-304.275813950724</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2">
-        <f>ABS(B5-C5)</f>
-        <v>304.275813950724</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3866</v>
-      </c>
-      <c r="F5" s="2">
-        <v>22</v>
-      </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="3">
-        <v>335</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="3">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="5">
-        <v>-304.27583126108198</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2">
-        <f>ABS(B10-C10)</f>
-        <v>304.27583126108198</v>
-      </c>
-      <c r="E10" s="2">
-        <v>201</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2">
-        <f>E11/E10</f>
-        <v>13.741293532338309</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="5">
-        <v>-304.27583126103599</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2">
-        <f>ABS(B11-C11)</f>
-        <v>304.27583126103599</v>
-      </c>
-      <c r="E11" s="2">
-        <v>2762</v>
-      </c>
-      <c r="F11" s="2">
-        <v>22</v>
-      </c>
-      <c r="G11" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B100792-F8E9-2145-A8FC-022CBCD50240}">
-  <dimension ref="A1:G11"/>
-  <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="144" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="3">
-        <v>335</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="3">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="5">
-        <v>-304.27613652339198</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="2">
-        <f>ABS(B4-C4)</f>
-        <v>304.27613652339198</v>
-      </c>
-      <c r="E4" s="2">
-        <v>234</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2">
-        <f>E5/E4</f>
-        <v>16.521367521367523</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2">
-        <v>-304.282028608556</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2">
-        <f>ABS(B5-C5)</f>
-        <v>304.282028608556</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3866</v>
-      </c>
-      <c r="F5" s="2">
-        <v>22</v>
-      </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="3">
-        <v>335</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="3">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="2">
-        <v>-304.27615367897698</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2">
-        <f>ABS(B10-C10)</f>
-        <v>304.27615367897698</v>
-      </c>
-      <c r="E10" s="2">
-        <v>193</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2">
-        <f>E11/E10</f>
-        <v>14.155440414507773</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="2">
-        <v>-304.27615367888802</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2">
-        <f>ABS(B11-C11)</f>
-        <v>304.27615367888802</v>
-      </c>
-      <c r="E11" s="2">
-        <v>2732</v>
-      </c>
-      <c r="F11" s="2">
-        <v>22</v>
-      </c>
-      <c r="G11" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE248C03-3D57-7F4D-B6B8-F4605338EEA9}">
   <dimension ref="A1:G80"/>
   <sheetViews>
@@ -11545,11 +10407,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64124B2-4DA6-A845-AF20-5E3DD1CD9D6F}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="187" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="187" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -12088,8 +10950,8 @@
   </sheetPr>
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="A26" zoomScale="135" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12125,13 +10987,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" s="3">
         <v>140</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D2" s="3">
         <v>37</v>
@@ -12160,23 +11022,23 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -12295,14 +11157,14 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B8" s="3">
         <f>B2</f>
         <v>140</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D8" s="3">
         <v>30</v>
@@ -12331,23 +11193,23 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -12430,7 +11292,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="10"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -12466,14 +11328,14 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B14" s="3">
         <f>B2</f>
         <v>140</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D14" s="3">
         <v>23</v>
@@ -12502,23 +11364,23 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -12613,7 +11475,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -12716,7 +11578,7 @@
         <v>74</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D25" s="3">
         <v>37</v>
@@ -12745,23 +11607,23 @@
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
@@ -12887,7 +11749,7 @@
         <v>74</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D31" s="3">
         <v>30</v>
@@ -12916,23 +11778,23 @@
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I32" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -13015,7 +11877,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
-      <c r="B35" s="10"/>
+      <c r="B35" s="9"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -13058,7 +11920,7 @@
         <v>74</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D37" s="3">
         <v>23</v>
@@ -13087,23 +11949,23 @@
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
@@ -13292,13 +12154,13 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B48" s="3">
         <v>33</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D48" s="3">
         <v>37</v>
@@ -13327,23 +12189,23 @@
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I49" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J49" s="2"/>
       <c r="K49" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
@@ -13462,14 +12324,14 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B54" s="3">
         <f>B48</f>
         <v>33</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D54" s="3">
         <v>30</v>
@@ -13498,23 +12360,23 @@
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I55" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G55" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J55" s="2"/>
       <c r="K55" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
@@ -13597,7 +12459,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
-      <c r="B58" s="10"/>
+      <c r="B58" s="9"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -13633,14 +12495,14 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B60" s="3">
         <f>B48</f>
         <v>33</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D60" s="3">
         <v>23</v>
@@ -13669,23 +12531,23 @@
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I61" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G61" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I61" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J61" s="2"/>
       <c r="K61" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
@@ -13807,7 +12669,7 @@
   </sheetPr>
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView topLeftCell="C34" zoomScale="141" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="141" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
@@ -13844,13 +12706,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" s="3">
         <v>140</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D2" s="3">
         <v>37</v>
@@ -13879,23 +12741,23 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -14013,14 +12875,14 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B8" s="3">
         <f>B2</f>
         <v>140</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D8" s="3">
         <v>30</v>
@@ -14049,23 +12911,23 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -14148,7 +13010,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="10"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -14184,14 +13046,14 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B14" s="3">
         <f>B2</f>
         <v>140</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D14" s="3">
         <v>23</v>
@@ -14220,23 +13082,23 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -14331,7 +13193,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -14434,7 +13296,7 @@
         <v>74</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D25" s="3">
         <v>37</v>
@@ -14463,23 +13325,23 @@
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
@@ -14605,7 +13467,7 @@
         <v>74</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D31" s="3">
         <v>30</v>
@@ -14634,23 +13496,23 @@
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I32" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -14775,7 +13637,7 @@
         <v>74</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D37" s="3">
         <v>23</v>
@@ -14804,23 +13666,23 @@
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
@@ -15009,13 +13871,13 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B48" s="3">
         <v>33</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D48" s="3">
         <v>37</v>
@@ -15044,23 +13906,23 @@
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I49" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J49" s="2"/>
       <c r="K49" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
@@ -15179,14 +14041,14 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B54" s="3">
         <f>B48</f>
         <v>33</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D54" s="3">
         <v>30</v>
@@ -15215,23 +14077,23 @@
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I55" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G55" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J55" s="2"/>
       <c r="K55" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
@@ -15314,7 +14176,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
-      <c r="B58" s="10"/>
+      <c r="B58" s="9"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -15350,14 +14212,14 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B60" s="3">
         <f>B48</f>
         <v>33</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D60" s="3">
         <v>23</v>
@@ -15386,23 +14248,23 @@
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I61" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="G61" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I61" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="J61" s="2"/>
       <c r="K61" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
removed large file from last commit
</commit_message>
<xml_diff>
--- a/gau_bm_new.xlsx
+++ b/gau_bm_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aodongliu/LiGroup/gaussian/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391BA933-56C0-7641-B245-38F3980806E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2A57E5-CF4B-3E44-9959-D6AA6F26CDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="13" xr2:uid="{FDC61512-9885-E840-A5B5-8D65FB928F9E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{FDC61512-9885-E840-A5B5-8D65FB928F9E}"/>
   </bookViews>
   <sheets>
     <sheet name="COH2 NEW" sheetId="18" r:id="rId1"/>
@@ -8746,7 +8746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B100792-F8E9-2145-A8FC-022CBCD50240}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="144" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="144" workbookViewId="0">
       <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
@@ -10950,8 +10950,8 @@
   </sheetPr>
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="135" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="135" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>